<commit_message>
1.comorbidity static coding 2.year base stat 3.beers criteria filtering ..ing
</commit_message>
<xml_diff>
--- a/condition_inform.xlsx
+++ b/condition_inform.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="condition" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,125 +16,137 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+  <si>
+    <t>Cardiac arrhythmias</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Congestive Heart failure</t>
+  </si>
+  <si>
+    <t>319825, 314378, 439696, 439694, 4110961, 4163710, 4190773, 318773, 321319, 320746, 316139, 4172864</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COPD</t>
+  </si>
+  <si>
+    <t>Coronary heart disease</t>
+  </si>
+  <si>
+    <t>Depression</t>
+  </si>
+  <si>
+    <t>Diabetes mellitus</t>
+  </si>
+  <si>
+    <t>Hyperlipidemia</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>320128, 442604, 201313, 195556, 319826</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liver disease</t>
+  </si>
+  <si>
+    <t>4012113, 24966, 4237824, 22340, 201612, 4026136, 4059298, 4055225, 4059299, 4058695, 4245975, 200763, 4267417, 4059290, 4058696, 194417, 4240725, 4277276, 192680, 196455, 194984, 42537742</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lymphoma</t>
+  </si>
+  <si>
+    <t>4038835, 4147411, 4003830, 4212994, 4038838, 4003834, 437233, 4094548, 4147164</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metastatic cancer</t>
+  </si>
+  <si>
+    <t>318096, 4147162, 432851, 443392</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Myocardial infarction</t>
+  </si>
+  <si>
+    <t>312327, 4108217</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Osteoarthritis</t>
+  </si>
+  <si>
+    <t>75897, 4079749, 4079750</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Osteoporosis</t>
+  </si>
+  <si>
+    <t>40480160, 80502, 45766159</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Renal failure</t>
+  </si>
+  <si>
+    <t>Solid tumor without metastasis</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>443454, 381316</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>condition_concept_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>condition_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>318448, 320744, 316135, 4057008, 321042, 313792, 4068155, 44784217, 444070, 4169095, 4262562, 4009798, 4032241, 45766277</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Asthma</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Cardiac arrhythmias</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>318448, 320744, 316135, 4057008, 321042, 313792, 4068155, 44784217, 444070, 4169095, 4262562, 4009798, 4032241, 45766277</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Congestive Heart failure</t>
-  </si>
-  <si>
-    <t>319825, 314378, 439696, 439694, 4110961, 4163710, 4190773, 318773, 321319, 320746, 316139, 4172864</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>COPD</t>
-  </si>
-  <si>
-    <t>Coronary heart disease</t>
-  </si>
-  <si>
-    <t>Depression</t>
-  </si>
-  <si>
     <t>4332994, 439254, 35622934, 440383, 4098302, 433440, 4338031, 436677</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Diabetes mellitus</t>
+    <t>443919, 439695, 46271022, 192359, 197921, 4301680, 4032243, 42539502, 4019967</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4155171, 256633, 437498, 140950, 135750, 134290, 25189, 434588, 4247836, 31509, 432833, 4095312, 435190, 439746, 436045, 443389, 26638, 196044, 443397, 197500, 438699, 74582, 40481902, 4095432, 197806, 194589, 199754, 4116238, 443389, 442131, 259748, 26052, 4177112, 4311499, 438368, 438693, 443389, 4180312, 76914, 141232, 4033891, 434584, 376918, 376918, 376647, 4162253, 195197, 196048, 196359, 4162860, 45770892, 200051, 201238, 36715801, 195483, 200962, 433716, 197507, 198985, 195480, 200054, 196360, 76349, 442131, 4002340, 380055, 4247822, 133424, 198104, 133420, 4114221, 4094409</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>man</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>woman</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>201254, 201826, 4327944, 201820</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hyperlipidemia</t>
-  </si>
-  <si>
-    <t>Hypertension</t>
-  </si>
-  <si>
-    <t>320128, 442604, 201313, 195556, 319826</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liver disease</t>
-  </si>
-  <si>
-    <t>4012113, 24966, 4237824, 22340, 201612, 4026136, 4059298, 4055225, 4059299, 4058695, 4245975, 200763, 4267417, 4059290, 4058696, 194417, 4240725, 4277276, 192680, 196455, 194984, 42537742</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lymphoma</t>
-  </si>
-  <si>
-    <t>4038835, 4147411, 4003830, 4212994, 4038838, 4003834, 437233, 4094548, 4147164</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Metastatic cancer</t>
-  </si>
-  <si>
-    <t>318096, 4147162, 432851, 443392</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Myocardial infarction</t>
-  </si>
-  <si>
-    <t>312327, 4108217</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Osteoarthritis</t>
-  </si>
-  <si>
-    <t>75897, 4079749, 4079750</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Osteoporosis</t>
-  </si>
-  <si>
-    <t>40480160, 80502, 45766159</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Renal failure</t>
-  </si>
-  <si>
-    <t>443919, 439695, 46271022, 192359, 197921, 4301680, 4032243, 42539502, 4019967</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solid tumor without metastasis</t>
-  </si>
-  <si>
-    <t>4155171, 256633, 437498, 140950, 135750, 134290, 25189, 434588, 4247836, 31509, 432833, 4095312, 435190, 439746, 436045, 443389, 26638, 196044, 443397, 197500, 438699, 74582, 40481902, 4095432, 197806, 194589, 199754, 4116238, 443389, 442131, 259748, 26052, 4177112, 4311499, 438368, 438693, 443389, 4180312, 76914, 141232, 4033891, 434584, 376918, 376918, 376647, 4162253, 195197, 196048, 196359, 4162860, 45770892, 200051, 201238, 36715801, 195483, 200962, 433716, 197507, 198985, 195480, 200054, 196360, 76349, 442131, 4002340, 380055, 4247822, 133424, 198104, 133420, 4114221, 4094409</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stroke</t>
-  </si>
-  <si>
-    <t>443454, 381316</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>condition_concept_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>condition_name</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -142,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +185,12 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -188,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -211,13 +229,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -229,6 +275,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,26 +589,26 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.25" customWidth="1"/>
+    <col min="2" max="2" width="255.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2">
         <v>317009</v>
@@ -561,23 +616,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>255573</v>
@@ -585,7 +640,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>315286</v>
@@ -593,23 +648,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>437530</v>
@@ -617,98 +672,557 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C2:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="C2:J23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="4">
+        <v>32007</v>
+      </c>
+      <c r="D4">
+        <f>ROUND(C4/$C$23*100,2)</f>
+        <v>2.86</v>
+      </c>
+      <c r="F4" s="4">
+        <v>13160</v>
+      </c>
+      <c r="G4">
+        <f>ROUND(F4/$C$23*100,2)</f>
+        <v>1.18</v>
+      </c>
+      <c r="I4" s="4">
+        <v>18847</v>
+      </c>
+      <c r="J4">
+        <f>ROUND(I4/$C$23*100,2)</f>
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="5">
+        <v>27000</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D20" si="0">ROUND(C5/$C$23*100,2)</f>
+        <v>2.41</v>
+      </c>
+      <c r="F5" s="5">
+        <v>13343</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G21" si="1">ROUND(F5/$C$23*100,2)</f>
+        <v>1.19</v>
+      </c>
+      <c r="I5" s="5">
+        <v>13657</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J21" si="2">ROUND(I5/$C$23*100,2)</f>
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="5">
+        <v>32883</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2.94</v>
+      </c>
+      <c r="F6" s="5">
+        <v>15486</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1.38</v>
+      </c>
+      <c r="I6" s="5">
+        <v>17397</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="5">
+        <v>55534</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4.96</v>
+      </c>
+      <c r="F7" s="5">
+        <v>45201</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>4.04</v>
+      </c>
+      <c r="I7" s="5">
+        <v>10333</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="5">
+        <v>13725</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.23</v>
+      </c>
+      <c r="F8" s="5">
+        <v>6985</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.62</v>
+      </c>
+      <c r="I8" s="5">
+        <v>6740</v>
+      </c>
+      <c r="J8">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="5">
+        <v>36251</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3.24</v>
+      </c>
+      <c r="F9" s="5">
+        <v>9406</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.84</v>
+      </c>
+      <c r="I9" s="5">
+        <v>26845</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="5">
+        <v>826</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>401</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="I10" s="5">
+        <v>425</v>
+      </c>
+      <c r="J10">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="5">
+        <v>22976</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="F11" s="5">
+        <v>10008</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.89</v>
+      </c>
+      <c r="I11" s="5">
+        <v>12968</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="5">
+        <v>323004</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>28.87</v>
+      </c>
+      <c r="F12" s="5">
+        <v>140665</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>12.57</v>
+      </c>
+      <c r="I12" s="5">
+        <v>182339</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="5">
+        <v>21472</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.92</v>
+      </c>
+      <c r="F13" s="5">
+        <v>11689</v>
+      </c>
+      <c r="G13">
+        <v>1.05</v>
+      </c>
+      <c r="I13" s="5">
+        <v>9783</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="5">
+        <v>8360</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="F14" s="5">
+        <v>4797</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.43</v>
+      </c>
+      <c r="I14" s="5">
+        <v>3563</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="5">
+        <v>1680</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="F15" s="5">
+        <v>878</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="I15" s="5">
+        <v>802</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="5">
+        <v>30634</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>2.74</v>
+      </c>
+      <c r="F16" s="5">
+        <v>18408</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1.65</v>
+      </c>
+      <c r="I16" s="5">
+        <v>12226</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="5">
+        <v>29264</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>2.62</v>
+      </c>
+      <c r="F17" s="5">
+        <v>5325</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+      <c r="I17" s="5">
+        <v>23939</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="5">
+        <v>62521</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>5.59</v>
+      </c>
+      <c r="F18" s="5">
+        <v>9211</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0.82</v>
+      </c>
+      <c r="I18" s="5">
+        <v>53310</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="5">
+        <v>50034</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>4.47</v>
+      </c>
+      <c r="F19" s="5">
+        <v>29772</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>2.66</v>
+      </c>
+      <c r="I19" s="5">
+        <v>20262</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="5">
+        <v>248057</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>22.17</v>
+      </c>
+      <c r="F20" s="5">
+        <v>159692</v>
+      </c>
+      <c r="G20">
+        <v>14.28</v>
+      </c>
+      <c r="I20" s="5">
+        <v>88365</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="5">
+        <v>122523</v>
+      </c>
+      <c r="D21">
+        <v>10.96</v>
+      </c>
+      <c r="F21" s="5">
+        <v>65268</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>5.83</v>
+      </c>
+      <c r="I21" s="5">
+        <v>57255</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>5.12</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f>SUM(C4:C21)</f>
+        <v>1118751</v>
+      </c>
+      <c r="D23">
+        <f>SUM(D4:D21)</f>
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <f>SUM(F4:F21)</f>
+        <v>559695</v>
+      </c>
+      <c r="G23">
+        <f>SUM(G4:G21)</f>
+        <v>50.029999999999994</v>
+      </c>
+      <c r="I23">
+        <f>SUM(I4:I21)</f>
+        <v>559056</v>
+      </c>
+      <c r="J23">
+        <f>SUM(J4:J21)</f>
+        <v>49.97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="I2:J2"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -718,7 +1232,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
chi sqare / t-test / comorbidity list counting
</commit_message>
<xml_diff>
--- a/condition_inform.xlsx
+++ b/condition_inform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="26955" windowHeight="12570"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="26955" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Cardiac arrhythmias</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -35,118 +35,156 @@
     <t>Coronary heart disease</t>
   </si>
   <si>
+    <t>Hyperlipidemia</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>320128, 442604, 201313, 195556, 319826</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liver disease</t>
+  </si>
+  <si>
+    <t>Lymphoma</t>
+  </si>
+  <si>
+    <t>4038835, 4147411, 4003830, 4212994, 4038838, 4003834, 437233, 4094548, 4147164</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metastatic cancer</t>
+  </si>
+  <si>
+    <t>318096, 4147162, 432851, 443392</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Myocardial infarction</t>
+  </si>
+  <si>
+    <t>312327, 4108217</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Osteoarthritis</t>
+  </si>
+  <si>
+    <t>75897, 4079749, 4079750</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Osteoporosis</t>
+  </si>
+  <si>
+    <t>40480160, 80502, 45766159</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Renal failure</t>
+  </si>
+  <si>
+    <t>Solid tumor without metastasis</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>443454, 381316</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>condition_concept_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>condition_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>318448, 320744, 316135, 4057008, 321042, 313792, 4068155, 44784217, 444070, 4169095, 4262562, 4009798, 4032241, 45766277</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Asthma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4332994, 439254, 35622934, 440383, 4098302, 433440, 4338031, 436677</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>443919, 439695, 46271022, 192359, 197921, 4301680, 4032243, 42539502, 4019967</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4155171, 256633, 437498, 140950, 135750, 134290, 25189, 434588, 4247836, 31509, 432833, 4095312, 435190, 439746, 436045, 443389, 26638, 196044, 443397, 197500, 438699, 74582, 40481902, 4095432, 197806, 194589, 199754, 4116238, 443389, 442131, 259748, 26052, 4177112, 4311499, 438368, 438693, 443389, 4180312, 76914, 141232, 4033891, 434584, 376918, 376918, 376647, 4162253, 195197, 196048, 196359, 4162860, 45770892, 200051, 201238, 36715801, 195483, 200962, 433716, 197507, 198985, 195480, 200054, 196360, 76349, 442131, 4002340, 380055, 4247822, 133424, 198104, 133420, 4114221, 4094409</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>man</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>woman</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diabetes mellitus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Depression</t>
-  </si>
-  <si>
-    <t>Diabetes mellitus</t>
-  </si>
-  <si>
-    <t>Hyperlipidemia</t>
-  </si>
-  <si>
-    <t>Hypertension</t>
-  </si>
-  <si>
-    <t>320128, 442604, 201313, 195556, 319826</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liver disease</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>201254, 201826, 4327944, 201820</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>4012113, 24966, 4237824, 22340, 201612, 4026136, 4059298, 4055225, 4059299, 4058695, 4245975, 200763, 4267417, 4059290, 4058696, 194417, 4240725, 4277276, 192680, 196455, 194984, 42537742</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Lymphoma</t>
-  </si>
-  <si>
-    <t>4038835, 4147411, 4003830, 4212994, 4038838, 4003834, 437233, 4094548, 4147164</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Metastatic cancer</t>
-  </si>
-  <si>
-    <t>318096, 4147162, 432851, 443392</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Myocardial infarction</t>
-  </si>
-  <si>
-    <t>312327, 4108217</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Osteoarthritis</t>
-  </si>
-  <si>
-    <t>75897, 4079749, 4079750</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Osteoporosis</t>
-  </si>
-  <si>
-    <t>40480160, 80502, 45766159</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Renal failure</t>
-  </si>
-  <si>
-    <t>Solid tumor without metastasis</t>
-  </si>
-  <si>
-    <t>Stroke</t>
-  </si>
-  <si>
-    <t>443454, 381316</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>condition_concept_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>condition_name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>318448, 320744, 316135, 4057008, 321042, 313792, 4068155, 44784217, 444070, 4169095, 4262562, 4009798, 4032241, 45766277</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Asthma</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>4332994, 439254, 35622934, 440383, 4098302, 433440, 4338031, 436677</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>443919, 439695, 46271022, 192359, 197921, 4301680, 4032243, 42539502, 4019967</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>4155171, 256633, 437498, 140950, 135750, 134290, 25189, 434588, 4247836, 31509, 432833, 4095312, 435190, 439746, 436045, 443389, 26638, 196044, 443397, 197500, 438699, 74582, 40481902, 4095432, 197806, 194589, 199754, 4116238, 443389, 442131, 259748, 26052, 4177112, 4311499, 438368, 438693, 443389, 4180312, 76914, 141232, 4033891, 434584, 376918, 376918, 376647, 4162253, 195197, 196048, 196359, 4162860, 45770892, 200051, 201238, 36715801, 195483, 200962, 433716, 197507, 198985, 195480, 200054, 196360, 76349, 442131, 4002340, 380055, 4247822, 133424, 198104, 133420, 4114221, 4094409</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>total</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>man</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>woman</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>201254, 201826, 4327944, 201820</t>
+    <t>금</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>화</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>목</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오전</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오후</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나오는날 기준</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전명훈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>황지영</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -192,7 +230,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +240,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,7 +307,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -283,6 +327,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -588,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -600,15 +647,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2">
         <v>317009</v>
@@ -619,7 +666,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -648,23 +695,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>437530</v>
@@ -672,82 +719,82 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -759,30 +806,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J23"/>
+  <dimension ref="C2:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="C2:J23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C2" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="4">
         <v>32007</v>
       </c>
@@ -805,7 +852,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="5" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="5">
         <v>27000</v>
       </c>
@@ -828,7 +875,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="6" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="5">
         <v>32883</v>
       </c>
@@ -851,7 +898,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="7" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="5">
         <v>55534</v>
       </c>
@@ -874,7 +921,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="5">
         <v>13725</v>
       </c>
@@ -896,7 +943,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="5">
         <v>36251</v>
       </c>
@@ -919,7 +966,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="10" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="5">
         <v>826</v>
       </c>
@@ -941,7 +988,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="5">
         <v>22976</v>
       </c>
@@ -964,7 +1011,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="12" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="5">
         <v>323004</v>
       </c>
@@ -987,7 +1034,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="13" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="5">
         <v>21472</v>
       </c>
@@ -1009,7 +1056,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="5">
         <v>8360</v>
       </c>
@@ -1032,7 +1079,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="5">
         <v>1680</v>
       </c>
@@ -1055,7 +1102,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="16" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="5">
         <v>30634</v>
       </c>
@@ -1077,8 +1124,15 @@
         <f t="shared" si="2"/>
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="5">
         <v>29264</v>
       </c>
@@ -1100,8 +1154,20 @@
         <f t="shared" si="2"/>
         <v>2.14</v>
       </c>
-    </row>
-    <row r="18" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M17" t="s">
+        <v>38</v>
+      </c>
+      <c r="N17" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="5">
         <v>62521</v>
       </c>
@@ -1123,8 +1189,23 @@
         <f t="shared" si="2"/>
         <v>4.7699999999999996</v>
       </c>
-    </row>
-    <row r="19" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" t="s">
+        <v>44</v>
+      </c>
+      <c r="N18" t="s">
+        <v>45</v>
+      </c>
+      <c r="O18" t="s">
+        <v>44</v>
+      </c>
+      <c r="P18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="5">
         <v>50034</v>
       </c>
@@ -1146,8 +1227,23 @@
         <f t="shared" si="2"/>
         <v>1.81</v>
       </c>
-    </row>
-    <row r="20" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" t="s">
+        <v>45</v>
+      </c>
+      <c r="N19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C20" s="5">
         <v>248057</v>
       </c>
@@ -1169,7 +1265,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="21" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="5">
         <v>122523</v>
       </c>
@@ -1191,7 +1287,7 @@
         <v>5.12</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C23">
         <f>SUM(C4:C21)</f>
         <v>1118751</v>
@@ -1218,10 +1314,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L16:P16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>